<commit_message>
Imports optimization and fixes
</commit_message>
<xml_diff>
--- a/blanksheet.xlsx
+++ b/blanksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsingh369\OneDrive - DXC Production\Documents\Python Projects\Incident Report Auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399B0836-9B94-49D8-8116-CFF71E0EC826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8066BDB2-8137-4877-B63C-2DB5C61AB97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2742FB5E-273A-472B-9597-07F697A093FF}"/>
   </bookViews>
@@ -502,6 +502,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016D910029B5B54439B5705A83A538354" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9132474e6ce3f27a7c992033cf1d5b5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3cd43e3-3947-4e85-aab1-553ab88ad72a" xmlns:ns3="39f1daab-f413-4c9e-94ea-95b7a1426ebc" xmlns:ns4="168e0357-5b39-4600-91c2-bfff6e896513" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef9fc6e2d363479c3c3fdcc41ce0ce5f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="a3cd43e3-3947-4e85-aab1-553ab88ad72a"/>
@@ -755,15 +764,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B6A52C-3606-4F4A-8A4C-053EF3B8F05E}">
   <ds:schemaRefs>
@@ -783,6 +783,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FAE148-F11D-4CE8-B210-67F77862F0CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2075178-18B2-4C1D-8DD4-D806EEE3B5AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -800,12 +808,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FAE148-F11D-4CE8-B210-67F77862F0CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changes to sso login process and excel sheet activities
</commit_message>
<xml_diff>
--- a/blanksheet.xlsx
+++ b/blanksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsingh369\OneDrive - DXC Production\Documents\Python Projects\Incident Report Auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8066BDB2-8137-4877-B63C-2DB5C61AB97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787037AC-9949-4BF1-996A-3F4BF0360CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2742FB5E-273A-472B-9597-07F697A093FF}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,22 +60,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="6"/>
+      <color rgb="FF000099"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0E0E0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDF3FE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -83,14 +112,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD9D9D9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF708090"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC9C9C9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF708090"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFC9C9C9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFC9C9C9"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFC9C9C9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF708090"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFC9C9C9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF708090"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD9D9D9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,15 +519,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD38FE19-F0AB-4EA0-B8FF-2B36BA2220E8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="3" width="10.6328125" style="3"/>
+    <col min="4" max="4" width="50.6328125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="25.6328125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.6328125" style="3"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -502,15 +795,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016D910029B5B54439B5705A83A538354" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9132474e6ce3f27a7c992033cf1d5b5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3cd43e3-3947-4e85-aab1-553ab88ad72a" xmlns:ns3="39f1daab-f413-4c9e-94ea-95b7a1426ebc" xmlns:ns4="168e0357-5b39-4600-91c2-bfff6e896513" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef9fc6e2d363479c3c3fdcc41ce0ce5f" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="a3cd43e3-3947-4e85-aab1-553ab88ad72a"/>
@@ -764,6 +1048,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B6A52C-3606-4F4A-8A4C-053EF3B8F05E}">
   <ds:schemaRefs>
@@ -783,14 +1076,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FAE148-F11D-4CE8-B210-67F77862F0CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2075178-18B2-4C1D-8DD4-D806EEE3B5AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -808,4 +1093,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04FAE148-F11D-4CE8-B210-67F77862F0CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>